<commit_message>
graphs in fammily budget:: by sergio giraldo @ 20230305T1428CET, gpg signed
</commit_message>
<xml_diff>
--- a/excel/ByRow-ByColumn-Lambda-Helper.xlsx
+++ b/excel/ByRow-ByColumn-Lambda-Helper.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/GK47LX/source/office/excel/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5840D9BB-F855-6046-B410-B827218FBFB3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{30DBFF74-9A9C-2C45-A1DD-AEE87B88F7FB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="20440" xr2:uid="{0ACB132C-7219-4B66-ACBB-64BA10C47BDC}"/>
   </bookViews>
@@ -55,7 +55,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="24">
   <si>
     <t>Jan</t>
   </si>
@@ -169,9 +169,6 @@
   </si>
   <si>
     <t>Employees</t>
-  </si>
-  <si>
-    <t>How You Can Actually Use the NEW Excel BYROW &amp; BYCOL Functions - YouTube</t>
   </si>
 </sst>
 </file>
@@ -638,7 +635,7 @@
   <dimension ref="A1:P19"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="P12" sqref="P12"/>
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
@@ -740,9 +737,7 @@
       <c r="M5" s="2">
         <v>1495</v>
       </c>
-      <c r="P5" s="5" t="s">
-        <v>24</v>
-      </c>
+      <c r="P5" s="5"/>
     </row>
     <row r="6" spans="1:16">
       <c r="A6" s="1" t="s">
@@ -1044,9 +1039,6 @@
       </c>
     </row>
   </sheetData>
-  <hyperlinks>
-    <hyperlink ref="P5" r:id="rId1" display="https://www.youtube.com/watch?v=YqaEJiwJj2I" xr:uid="{DCD8F4DF-14FF-DB41-A694-0BE66A8A8A6E}"/>
-  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -1061,6 +1053,12 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100CF978176D7B6BC41934141C52985821B" ma:contentTypeVersion="11" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="c061e5688a2a9e5cc0c2876f63727f59">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="8602ebc8-99ea-4c12-aabd-36e02eea0ec4" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="3a3aeb9b15768c7faefdb57d8fe7a3b3" ns2:_="">
     <xsd:import namespace="8602ebc8-99ea-4c12-aabd-36e02eea0ec4"/>
@@ -1250,12 +1248,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D6669608-E3C8-4D28-84EB-82B3FB030CA0}">
   <ds:schemaRefs>
@@ -1265,6 +1257,15 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C5CE1196-3A32-4E87-BDCC-1CCE58FB8EB3}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3DD8DF6F-A7A4-45FF-9AF4-F5F362A22420}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -1280,13 +1281,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C5CE1196-3A32-4E87-BDCC-1CCE58FB8EB3}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>